<commit_message>
modifica file performance e modifica documentazione
</commit_message>
<xml_diff>
--- a/performance/performance_es_1.xlsx
+++ b/performance/performance_es_1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luigi\SNA\performance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CA09FE4-9A07-4B2B-B7C7-7B6D7D0AC1FE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7311B204-5EF4-4518-B3EF-B68FD4078AFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>ALGORITMO</t>
   </si>
@@ -91,6 +91,12 @@
   </si>
   <si>
     <t>necessario pc con 8+ gb di ram</t>
+  </si>
+  <si>
+    <t>hierarchical naïve (MARIO)</t>
+  </si>
+  <si>
+    <t>satura la memoria, tempo infinito</t>
   </si>
 </sst>
 </file>
@@ -408,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -534,6 +540,14 @@
         <v>7253.1139056682496</v>
       </c>
     </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Final Es 3 mod and excel mod
</commit_message>
<xml_diff>
--- a/performance/performance_es_1.xlsx
+++ b/performance/performance_es_1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luigi\SNA\performance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\albc\Alberto\Uni\Social Network\SNA\performance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7311B204-5EF4-4518-B3EF-B68FD4078AFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10005AF-62DB-4919-A0B0-91D18A22881F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
   <si>
     <t>ALGORITMO</t>
   </si>
@@ -97,6 +97,48 @@
   </si>
   <si>
     <t>satura la memoria, tempo infinito</t>
+  </si>
+  <si>
+    <t>da calcolare il tempo( 1.5s)</t>
+  </si>
+  <si>
+    <t>da calcolare il tempo(40 min)</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>btw nayve</t>
+  </si>
+  <si>
+    <t>4 means Nayve</t>
+  </si>
+  <si>
+    <t>spectral 80% comp connessa</t>
+  </si>
+  <si>
+    <t>spectral 70% comp connessa</t>
+  </si>
+  <si>
+    <t>btw 50% comp connessa</t>
+  </si>
+  <si>
+    <t>btw 70% comp connessa</t>
+  </si>
+  <si>
+    <t>4 means opt(ALB)</t>
+  </si>
+  <si>
+    <t>btw parallel(ALB)</t>
+  </si>
+  <si>
+    <t>caricare pkl</t>
+  </si>
+  <si>
+    <t>link pkl</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/drive/folders/10g-AdWR3G9_fo3vCiGeoRuXzTAIylEBr?usp=sharing</t>
   </si>
 </sst>
 </file>
@@ -136,7 +178,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -414,22 +456,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.6328125" customWidth="1"/>
-    <col min="2" max="2" width="33.453125" customWidth="1"/>
-    <col min="3" max="3" width="27.36328125" customWidth="1"/>
-    <col min="4" max="4" width="13.36328125" customWidth="1"/>
-    <col min="5" max="5" width="25.81640625" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="33.42578125" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="25.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -476,7 +518,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -487,9 +529,12 @@
         <v>82966.5179359912</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
       </c>
       <c r="E3">
         <f>AVERAGE(F3:O3)</f>
@@ -526,7 +571,7 @@
         <v>4.1695647239684996</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -540,12 +585,111 @@
         <v>7253.1139056682496</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>